<commit_message>
Preparing for implementation of Genetic Algorithm.
</commit_message>
<xml_diff>
--- a/data/samples/tpm/F5.xlsx
+++ b/data/samples/tpm/F5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\oh\Academia\Computacion\Algorithms\Project\Back-\data\samples\tpm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026976C2-D798-43BA-9242-977425A60D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1501449-5755-427E-BDED-BCD17756420B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5052" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -32,12 +32,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -63,7 +71,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,604 +347,557 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E32"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>0</v>
+      </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>